<commit_message>
Added API to Fetch the filter data
</commit_message>
<xml_diff>
--- a/planisware_data_1.xlsx
+++ b/planisware_data_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakash.yadav\PycharmProjects\GPD_Flask_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24821F69-C48C-4F50-8EE6-FA7DD9348772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632188D2-02FF-4E91-85A0-B808B5075911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1836" yWindow="1764" windowWidth="20208" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -106,9 +106,6 @@
     <t>CT_FN</t>
   </si>
   <si>
-    <t>Withdrawn</t>
-  </si>
-  <si>
     <t>PH IIA</t>
   </si>
   <si>
@@ -164,6 +161,54 @@
   </si>
   <si>
     <t>P-Proposed</t>
+  </si>
+  <si>
+    <t>Biosimilars</t>
+  </si>
+  <si>
+    <t>Cardiovascular and Metabolic</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Neurosciemce &amp; Pain</t>
+  </si>
+  <si>
+    <t>RareDisease</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Launched</t>
+  </si>
+  <si>
+    <t>Pfizer Code</t>
+  </si>
+  <si>
+    <t>PF01</t>
+  </si>
+  <si>
+    <t>PF02</t>
+  </si>
+  <si>
+    <t>PF03</t>
+  </si>
+  <si>
+    <t>PF04</t>
+  </si>
+  <si>
+    <t>PF05</t>
+  </si>
+  <si>
+    <t>PF06</t>
+  </si>
+  <si>
+    <t>PF07</t>
+  </si>
+  <si>
+    <t>PF08</t>
   </si>
 </sst>
 </file>
@@ -171,7 +216,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -201,7 +246,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -224,16 +269,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +618,7 @@
     <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,13 +661,16 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -623,7 +685,7 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
@@ -649,13 +711,16 @@
       <c r="O2" t="s">
         <v>24</v>
       </c>
+      <c r="P2" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -673,7 +738,7 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -696,13 +761,16 @@
       <c r="O3" t="s">
         <v>24</v>
       </c>
+      <c r="P3" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -717,25 +785,25 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
         <v>20</v>
       </c>
       <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
         <v>30</v>
-      </c>
-      <c r="M4" t="s">
-        <v>31</v>
       </c>
       <c r="N4" t="s">
         <v>24</v>
@@ -743,16 +811,19 @@
       <c r="O4" t="s">
         <v>23</v>
       </c>
+      <c r="P4" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2">
         <v>44440.333333333343</v>
@@ -764,25 +835,25 @@
         <v>15</v>
       </c>
       <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
       </c>
       <c r="K5" t="s">
         <v>20</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N5" t="s">
         <v>24</v>
@@ -790,16 +861,19 @@
       <c r="O5" t="s">
         <v>23</v>
       </c>
+      <c r="P5" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2">
         <v>44571.333333333343</v>
@@ -811,22 +885,22 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
       </c>
       <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s">
         <v>34</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
       </c>
       <c r="K6" t="s">
         <v>20</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
         <v>22</v>
@@ -837,16 +911,19 @@
       <c r="O6" t="s">
         <v>24</v>
       </c>
+      <c r="P6" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2">
         <v>44356.333333333343</v>
@@ -855,16 +932,16 @@
         <v>44984.833333333343</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s">
         <v>41</v>
-      </c>
-      <c r="I7" t="s">
-        <v>42</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
@@ -873,10 +950,10 @@
         <v>20</v>
       </c>
       <c r="L7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" t="s">
         <v>43</v>
-      </c>
-      <c r="M7" t="s">
-        <v>44</v>
       </c>
       <c r="N7" t="s">
         <v>23</v>
@@ -884,16 +961,19 @@
       <c r="O7" t="s">
         <v>24</v>
       </c>
+      <c r="P7" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2">
         <v>44348.333333333343</v>
@@ -902,16 +982,16 @@
         <v>45701.833333333343</v>
       </c>
       <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
         <v>40</v>
       </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>41</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
       </c>
       <c r="J8" t="s">
         <v>25</v>
@@ -920,10 +1000,10 @@
         <v>20</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N8" t="s">
         <v>24</v>
@@ -931,16 +1011,19 @@
       <c r="O8" t="s">
         <v>24</v>
       </c>
+      <c r="P8" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2">
         <v>43355.333333333343</v>
@@ -949,19 +1032,19 @@
         <v>44728.833333333343</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" t="s">
         <v>41</v>
       </c>
-      <c r="I9" t="s">
-        <v>42</v>
-      </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" t="s">
         <v>20</v>
@@ -978,16 +1061,19 @@
       <c r="O9" t="s">
         <v>23</v>
       </c>
+      <c r="P9" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2">
         <v>43635.333333333343</v>
@@ -996,16 +1082,16 @@
         <v>45474.833333333343</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" t="s">
         <v>41</v>
-      </c>
-      <c r="I10" t="s">
-        <v>42</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
@@ -1014,10 +1100,10 @@
         <v>20</v>
       </c>
       <c r="L10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N10" t="s">
         <v>24</v>
@@ -1025,16 +1111,19 @@
       <c r="O10" t="s">
         <v>24</v>
       </c>
+      <c r="P10" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2">
         <v>44377.333333333343</v>
@@ -1043,16 +1132,16 @@
         <v>44811.833333333343</v>
       </c>
       <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
         <v>40</v>
       </c>
-      <c r="G11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>41</v>
-      </c>
-      <c r="I11" t="s">
-        <v>42</v>
       </c>
       <c r="J11" t="s">
         <v>25</v>
@@ -1061,16 +1150,19 @@
         <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N11" t="s">
         <v>24</v>
       </c>
       <c r="O11" t="s">
         <v>23</v>
+      </c>
+      <c r="P11" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>